<commit_message>
Included unstable housing in the dataset and increased prevalence of unsuppressed patients
</commit_message>
<xml_diff>
--- a/evaluation_results.xlsx
+++ b/evaluation_results.xlsx
@@ -1,38 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/djf2150/devel/panelViz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F596DB00-67B1-7F4F-A284-51443957312C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B72D6EF-E582-1244-8C86-8CCDA61FD43E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14200" yWindow="3280" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{CD715CD4-5639-CA48-BB31-51A1A9D0643E}"/>
+    <workbookView xWindow="13960" yWindow="9840" windowWidth="28040" windowHeight="17040" xr2:uid="{CD715CD4-5639-CA48-BB31-51A1A9D0643E}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient Selections" sheetId="1" r:id="rId1"/>
     <sheet name="Health-ITUES" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Participant</t>
   </si>
@@ -155,6 +149,57 @@
   </si>
   <si>
     <t>Mabel F</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>Q17</t>
   </si>
 </sst>
 </file>
@@ -508,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A321F009-B975-724B-96F1-661C673983C2}">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391F74D0-6072-5C41-A5F7-CFD1B8F8FCE7}">
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,56 +713,56 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>7</v>
-      </c>
-      <c r="J1">
-        <v>8</v>
-      </c>
-      <c r="K1">
-        <v>9</v>
-      </c>
-      <c r="L1">
-        <v>10</v>
-      </c>
-      <c r="M1">
-        <v>11</v>
-      </c>
-      <c r="N1">
-        <v>12</v>
-      </c>
-      <c r="O1">
-        <v>13</v>
-      </c>
-      <c r="P1">
-        <v>14</v>
-      </c>
-      <c r="Q1">
-        <v>15</v>
-      </c>
-      <c r="R1">
-        <v>16</v>
-      </c>
-      <c r="S1">
-        <v>17</v>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>